<commit_message>
Rename result Inconclusive to Non-Negative
CVDLS-154
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/specimen-results.xlsx
+++ b/tests/ExcelImport/workbooks/specimen-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7673057-7030-0240-92C0-56AB203B0F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218914F8-BF63-8F45-B4E1-1653A0704341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12520" yWindow="460" windowWidth="15320" windowHeight="17540" xr2:uid="{A40D6FB2-8C03-E045-B2A6-5AEE355AAA37}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Negative</t>
   </si>
   <si>
-    <t>Inconclusive</t>
-  </si>
-  <si>
     <t>Recommended</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>SpecimenQPCRResults9</t>
+  </si>
+  <si>
+    <t>Non-Negative</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,129 +543,129 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>